<commit_message>
base url parameter added
base url,update jupyter notebook  and new crisis message added
</commit_message>
<xml_diff>
--- a/Chatbot/evaluation/chatbot_responses_template.xlsx
+++ b/Chatbot/evaluation/chatbot_responses_template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>Question</t>
   </si>
@@ -19,7 +19,7 @@
     <t>Chat gpt 40</t>
   </si>
   <si>
-    <t>Mental_Health Chatbot</t>
+    <t>Mental Health Chatbot</t>
   </si>
   <si>
     <t>Gemini</t>
@@ -115,6 +115,270 @@
   </si>
   <si>
     <t>I’m sorry you’re going through this—panic attacks can feel terrifying, but you’re safe, and this will pass. Right now, focus on anchoring yourself in the present: name five things you can see, four you can touch, three you can hear, two you can smell, and one you can taste. This grounds your nervous system in reality. Slow your breathing—try inhaling for four counts, holding for four, and exhaling for six—to signal to your body that the danger isn’t real. If possible, place a hand over your heart and remind yourself, This is temporary. I am okay. Avoid judging the panic; it’s just your body’s overprotective alarm system. Once the intensity fades, drink some water and rest. Later, we can explore triggers or coping tools, but for now, just be gentle with yourself. You’re getting through it, moment by moment.</t>
+  </si>
+  <si>
+    <t>I can’t stop crying and I don’t know why.</t>
+  </si>
+  <si>
+    <t>I'm really sorry you're feeling this way. Crying without a clear reason can be overwhelming and confusing. It might be your mind or body processing something you haven’t fully recognized yet—stress, exhaustion, grief, loneliness, or even something biochemical like a hormonal imbalance or depression.
+You don’t have to go through this alone. Talking to someone you trust, like a friend, family member, or therapist, can help you feel more grounded and supported. If this keeps happening or feels too much to handle, it’s really important to reach out to a mental health professional—they can help you get to the root of it.
+Would you like to talk a bit about what’s been going on lately?</t>
+  </si>
+  <si>
+    <t>It sounds like you may be experiencing some emotional distress. Have you tried talking to a therapist or counselor about your feelings? They may be able to help you figure out the root cause of your crying and provide you with coping techniques. Would you like me to find the nearest therapists for you?</t>
+  </si>
+  <si>
+    <t>Oh, honey, that sounds really tough. It's okay to not know why you're feeling this way, but it's also understandable that you'd want to figure it out. Sometimes emotions just bubble up.
+Have you noticed anything else going on lately? Even small things like a change in your routine, a little less sleep than usual, or something someone said that might have stuck with you? Sometimes the reasons aren't obvious right away.
+Just know that it's alright to cry. It can be a way for your body to release emotions. If you feel overwhelmed or like this has been going on for a while, talking to someone might help. There are people who care and want to support you.</t>
+  </si>
+  <si>
+    <t>Sometimes our emotions need physical release before we can understand them, much like a storm that needs to pass before we can see clearly again. Your tears might be responding to something your conscious mind hasn't fully processed yet—accumulated stress, grief, or even emotional exhaustion that's been building beneath your awareness.
+Try to give yourself permission to cry without immediately needing to explain or fix it. Sit with the feeling, perhaps placing a hand on your heart or abdomen to offer yourself some physical comfort. Once the intensity subsides a bit, you might notice subtle clues about what's underneath these tears—perhaps a need that's gone unmet, a boundary that's been crossed, or simply the need for rest and care. The body often speaks in emotions before we have words for our experiences, so this crying may actually be an important message rather than something to stop.
+When you feel ready, what would feel like gentle care for yourself right now?</t>
+  </si>
+  <si>
+    <t>It’s okay to let the tears flow—sometimes they’re the heart’s way of releasing what the mind hasn’t fully processed yet. You don’t need a "reason" to justify this; emotions often surface when your body senses it’s finally safe enough to feel. Instead of fighting it, try offering yourself simple kindness: This is hard right now, and that’s alright. If you can, wrap yourself in a blanket, hold a warm mug, or sit quietly where you feel grounded. Tears can be a release of old stress, unresolved grief, or even exhaustion—no detective work needed today. Later, if you want to explore patterns (like when this happens or what follows), we can. But for now, just breathe through it. You’re not broken; you’re human.
+Would it feel comforting to name one gentle thing you could do for yourself in this moment?</t>
+  </si>
+  <si>
+    <t>I don’t think I matter to anyone.</t>
+  </si>
+  <si>
+    <t>I'm really sorry you're feeling this way. When you believe you don’t matter, it can make everything feel heavier and more painful—but that belief, as real as it feels, is not the truth.
+You *do* matter. Even if you can't see it right now, your presence has value. People may not always show it the way you need or expect, but that doesn't mean you're invisible or unimportant. Sometimes, when we’re hurting, our minds filter everything through pain, convincing us that we're alone or don’t belong. But those thoughts aren’t facts—they’re signs that something inside you is asking for care and connection.
+You’re not alone in this. You don’t have to carry it all by yourself. It’s okay to ask for help. You deserve to be seen, heard, and supported.
+Can I ask—has anything happened recently that made you feel this way more intensely?</t>
+  </si>
+  <si>
+    <t>I am here to talk to you and offer support. It may feel like you don't matter to anyone, but that is not true. You are valued and important. Have you considered talking to a therapist about these feelings? They can help you work through these thoughts and find ways to feel more connected and valued.</t>
+  </si>
+  <si>
+    <t>It sounds like you're going through a really tough time right now, feeling this profound sense of disconnection. It's important to acknowledge that these feelings of not mattering can be incredibly painful and isolating. Often, when we're feeling down or overwhelmed, our minds can play tricks on us, and we might start to focus on moments that seem to confirm these negative beliefs while overlooking the connections and care that might actually be present in our lives. Have there been any recent events or ongoing situations that might be contributing to these feelings? Sometimes exploring the roots of these thoughts can help us to see them more clearly and begin to challenge them. Remember, your feelings are valid, and it takes courage to acknowledge them.</t>
+  </si>
+  <si>
+    <t>That profound sense of not mattering cuts deeply into how we experience ourselves in the world. When we feel invisible or disposable to others, it creates a painful disconnect that colors everything else. What you're feeling isn't unusual, but it reflects your current perception rather than an objective truth about your place in others' lives.
+Our connections with others often operate beneath the surface of daily interactions. People may carry thoughts of you, be influenced by things you've said or done, or value your presence in ways they haven't expressed directly. Sometimes the people who matter most to us struggle to communicate that importance clearly. Your absence would create a void that others would feel, even if right now you can't see evidence of that. The challenge is that when we're feeling unimportant, we tend to interpret others' actions through that lens, creating a self-reinforcing cycle that's difficult to break from within.
+Can you think of even one small moment when someone responded to you in a way that suggested you mattered, even if it seemed insignificant at the time?</t>
+  </si>
+  <si>
+    <t>That thought—I don’t matter—carries such deep pain, and I want you to know it’s not a truth, but a reflection of how isolated or unseen you might feel right now. When we’re hurting, the mind can distort reality, convincing us we’re invisible to others. But your worth isn’t defined by how others show up (or don’t) for you. Try this: If someone I loved felt this way, what would I tell them? Often, we offer others the compassion we can’t yet give ourselves. You matter inherently—not because of what you do or provide, but simply because you exist. If you’re open to it, we could explore one small way to reconnect with your sense of value, like reaching out to someone who’s shown care before, or even writing a letter to your future self. You’re not alone in this darkness, even if it feels that way.
+Would you be willing to share what kind of support feels most missing right now? (No pressure—just know I’m here.)</t>
+  </si>
+  <si>
+    <t>I feel like giving up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'm really sorry you're feeling this way. It sounds like you’re carrying a lot right now, and it’s incredibly brave that you’re reaching out and sharing this—especially when things feel so heavy.
+Feeling like giving up is often a sign that you’re not wanting to end your life, but to end the pain. There *is* a difference—and there *is* help. You don’t have to go through this alone, and you don’t have to keep holding it all in.
+Please, if you’re in immediate danger or seriously thinking about hurting yourself, reach out right now to a crisis line or mental health professional. In the U.S., you can call or text **988** for the Suicide &amp; Crisis Lifeline. They’re there 24/7, and they *really do care*.
+You don’t need to have all the answers or explain everything. Just let someone in. One moment, one step, one conversation can be the start of something better—even if it doesn’t feel that way right now.
+I'm here to talk with you as much as you need. What you're feeling is valid—but it's not permanent. Would it be okay if I helped you find some support near you?
+</t>
+  </si>
+  <si>
+    <t>It sounds like you are going through a difficult time. Remember that you are not alone and there is always hope for things to get better. Have you considered talking to a therapist about these feelings? They can provide you with support and guidance to help you through this tough time.</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Detects crisis and provides helpline number&gt;&gt;</t>
+  </si>
+  <si>
+    <t>That exhaustion when you've been carrying too much for too long is profoundly real. When our inner resources are depleted, continuing forward can feel impossible, like trying to pour from an empty cup. This feeling of surrender isn't weakness—it's your mind and body signaling that something needs to change because the current path has become unsustainable.
+"Giving up" doesn't have to mean giving up on everything, but perhaps letting go of certain expectations, timelines, or ways of coping that no longer serve you. Sometimes what we need isn't to push harder but to release what's draining us. Consider what specifically feels too heavy right now. Is it possible to temporarily set down some responsibilities, adjust some expectations, or reach for support in a way you haven't before? When we're at this point, even a small shift in our burden can create enough space to find our footing again.
+What's one small thing you could release or pause right now to create even a tiny bit more breathing room for yourself?</t>
+  </si>
+  <si>
+    <t>I hear how much pain you’re in right now, and I want you to know that you don’t have to carry this alone. When the weight feels unbearable, it’s not a sign of weakness to reach for help—it’s an act of courage. You might not see a way forward yet, but that doesn’t mean one doesn’t exist. Let’s pause for a moment: What would it feel like to give yourself permission to set this heaviness down, even just for tonight? You don’t have to have answers right now. If the thought of tomorrow feels like too much, focus only on the next hour. Call a trusted friend, a crisis line, or even just stay here with me—you deserve to be met with care in this darkness. Your life matters, even if you can’t feel it right now.
+If you’re in immediate danger, please reach out to someone who can be with you—a hotline, a friend, or emergency services. You are worth that call.
+Would you let me walk with you through this? We can take it one breath at a time.</t>
+  </si>
+  <si>
+    <t>I’m exhausted all the time but can’t relax.</t>
+  </si>
+  <si>
+    <t>That sounds incredibly hard—being so tired yet unable to find rest is like being stuck in a loop that just drains you more. Emotional exhaustion, anxiety, and even depression can create exactly that feeling: your body is worn out, but your mind won’t shut off, so you never really get a break.
+This kind of exhaustion isn’t laziness or weakness—it's a signal. It’s your system trying to tell you that something needs attention, whether it’s emotional overload, stress, burnout, unresolved grief, or something deeper.
+You don’t have to fix everything at once. But it might help to start gently:
+Have you been able to take even a few minutes for quiet or deep breathing?
+Is there anyone in your life who makes you feel safe just being yourself—even for a short chat?
+Have you noticed any patterns in when you feel most overwhelmed?
+I can also help walk you through some calming techniques or grounding exercises, if that feels helpful. Would you like that?</t>
+  </si>
+  <si>
+    <t>There are many things you can try to help manage stress. Some suggestions include practicing relaxation techniques such as deep breathing or meditation, getting regular exercise, eating a healthy diet, and talking to a therapist or counselor. It's important to find what works best for you and to make self-care a priority.</t>
+  </si>
+  <si>
+    <t>That sounds incredibly frustrating and draining. To be constantly fatigued yet unable to find true rest creates a difficult cycle. Often, this kind of persistent exhaustion coupled with an inability to relax can be a sign that your body and mind are in a state of heightened tension. There might be underlying stress, worries, or even physiological factors that are keeping your nervous system activated, preventing you from fully unwinding even when you're physically still. Have you noticed any particular thoughts or situations that tend to ramp up this feeling of being unable to relax? Exploring those triggers might offer some clues about what's contributing to this persistent state of exhaustion without rest.</t>
+  </si>
+  <si>
+    <t>You're caught in that difficult paradox where your body and mind desperately need rest, yet your nervous system remains locked in a state of alertness that prevents true relaxation. This persistent tension often develops when we've been in survival mode for too long, creating a background hum of vigilance that's exhausting but hard to switch off.
+Rather than aiming directly for relaxation, which can sometimes increase the pressure you're feeling, try engaging in something absorbing that gently redirects your attention—perhaps a simple creative task, light movement, or even mundane activities like organizing a small space. These can serve as stepping stones between high alert and true rest. Your body needs signals that it's safe to stand down from constant readiness. Sometimes physical cues like warmth, weighted blankets, or specific breathing patterns can speak more directly to your nervous system than mental efforts alone.
+What have you noticed helps even slightly decrease your tension, even if it doesn't fully relax you?</t>
+  </si>
+  <si>
+    <t>What you’re describing—that relentless fatigue paired with an inability to unwind—suggests your nervous system may be stuck in a state of high alert, like an engine idling nonstop. This often happens when stress or unresolved emotions accumulate over time. Instead of pushing harder to "fix" it, try approaching yourself with curiosity: *When did I last feel truly at ease? What does my body need to feel safe right now?* Small, tangible steps can help—a 10-minute body scan (focusing on relaxing each muscle), a warm shower, or even just changing your environment (like stepping outside for fresh air). Your exhaustion is valid, and rest isn’t a reward for productivity—it’s a basic need. Let’s explore what barriers come up when you try to relax. Is it guilt? Racing thoughts? Something else? You deserve moments of peace.  
+Would it help to brainstorm one tiny ritual to signal to your body that it’s okay to rest?</t>
+  </si>
+  <si>
+    <t>Everything feels out of control right now.</t>
+  </si>
+  <si>
+    <t>When everything feels out of control, it can be deeply unsettling—like you're caught in a storm with no sense of where it's going or when it will stop. That feeling often comes when life throws too much at once, or when something inside you is trying to hold too many emotions without space to process them. In those moments, your mind and body go into survival mode, and it becomes hard to think clearly or feel grounded. What you're experiencing isn’t weakness—it’s a response to overwhelm. You don’t need to figure everything out right now. Sometimes, the first act of control is simply pausing, breathing, and recognizing that this moment—however painful—is not permanent. You are still here, and that matters. We can slow things down together. Can you tell me more about what’s been making things feel so out of control lately?</t>
+  </si>
+  <si>
+    <t>It's completely understandable to feel overwhelmed and like everything is out of control. Have you tried talking to a therapist about these feelings? They can help you work through your thoughts and find ways to cope with the stress and chaos. Would you like me to find the nearest therapists for you?</t>
+  </si>
+  <si>
+    <t>It's understandable that you're feeling overwhelmed when everything seems out of control. That sense of things being chaotic and unpredictable can create a lot of anxiety and unease. Often, when we experience this, it's helpful to identify the specific areas where you feel this lack of control. Is it related to work, relationships, personal goals, or perhaps a combination of things? Sometimes, by breaking down the larger feeling into smaller, more specific aspects, we can start to identify small steps you might be able to take, even tiny ones, to regain a sense of agency in those areas. Even focusing on what you can influence in the present moment can sometimes help to ground you amidst the feeling of everything else being in flux.</t>
+  </si>
+  <si>
+    <t>That sensation of life spiraling beyond your influence can be deeply unsettling, like trying to stand on shifting ground. When multiple aspects of life feel chaotic simultaneously, our natural desire for stability and predictability gets overwhelmed, creating that pervasive feeling that nothing is within your grasp.
+In these moments, it helps to deliberately narrow your focus to what is actually within your control, however small. Perhaps it's how you arrange your personal space, when you go to bed, or even just your breathing for the next minute. Creating even tiny islands of predictability can provide anchor points amid the turbulence. Remember that this acute feeling of chaos typically doesn't represent a permanent state—rather, it's often a transitional period where old patterns are breaking down before new ones have formed. Your sense of agency will gradually rebuild as you collect small experiences of influencing your immediate environment.
+What's one very small domain where you might still have some element of choice or control right now?</t>
+  </si>
+  <si>
+    <t>That sense of losing control is one of the most unsettling feelings—like the ground beneath you is shifting, and there’s nothing solid to hold onto. It makes complete sense that you’d feel overwhelmed. When the world or our inner world feels chaotic, our nervous system often reacts as if we’re in real danger, even if the threats aren’t physical.  
+Let’s start small: *What’s one thing within your control right now?* It might be as simple as adjusting your posture, choosing to drink a glass of water, or closing your eyes for three deep breaths. These tiny anchors can create a sense of stability when everything else feels unstable.  
+You don’t have to figure it all out at once. Sometimes, the healthiest response to chaos is to *pause*—to stop trying to grip tighter and instead ask, *How can I be kind to myself in this moment?*  
+Would it help to talk about what specifically feels most out of control? Or would you rather focus on grounding tools first? I’m here either way.</t>
+  </si>
+  <si>
+    <t>I feel like I’m all alone.</t>
+  </si>
+  <si>
+    <t>Feeling alone—especially when you’re hurting—can be one of the most painful experiences. It can make everything else feel heavier, like you’re carrying the weight of your world with no one to help hold it. Sometimes, even when people are technically around, it still feels like no one truly sees you or understands what you're going through. That sense of emotional isolation can grow quietly, especially if you've been strong for too long or have felt like a burden when reaching out. But just because you feel alone doesn’t mean you are unworthy of connection. Sometimes, it’s not about the number of people around you, but about whether you feel safe enough to be fully yourself with even one person. Right now, I want you to know I see you, and I’m here with you in this space. Would you feel comfortable telling me if there’s anyone in your life you’ve wanted to turn to but haven’t?</t>
+  </si>
+  <si>
+    <t>It's completely understandable to feel alone at times. But it's important to remember that you are never truly alone. There are people who care about you and support you. Have you considered talking to a therapist about these feelings? They can provide you with personalized support and guidance.</t>
+  </si>
+  <si>
+    <t>That feeling of being all alone can be incredibly isolating, and it's a really difficult emotion to carry. It's important to acknowledge that feeling and how heavy it can be. Sometimes, even when we are surrounded by people, we can still experience a deep sense of loneliness. This feeling might stem from a lack of meaningful connection, a feeling of not being understood, or perhaps a recent change in your social circumstances. Have there been any shifts in your relationships or social interactions lately that might be contributing to this feeling? Exploring what "alone" means to you in this moment can sometimes shed light on what kind of connection or support you might be longing for. Remember, acknowledging this feeling is the first step, and it doesn't mean you are truly alone in the broader sense.</t>
+  </si>
+  <si>
+    <t>That profound sense of aloneness can settle into the spaces between our ribs even when others are physically present. Loneliness isn't just about physical isolation - it's that painful awareness of a gap between the connection we crave and what we're experiencing. Even in a crowd, we can feel like we're watching life through glass, unable to truly be seen or understood.
+What makes this experience especially difficult is how it tends to turn inward - we start questioning whether something about us makes genuine connection impossible. In reality, meaningful connection often requires vulnerability that feels risky, especially if you've been hurt before. Consider that connection doesn't always need to be perfect or profound - sometimes small, authentic moments where you share something genuine or respond to another's humanity can create tiny bridges out of isolation. These small connections, while not solving everything, remind us that the walls between us and others aren't as impenetrable as they sometimes feel.
+Is there someone in your life, even someone you don't know well, with whom you might share even a small authentic moment or conversation?</t>
+  </si>
+  <si>
+    <t>The weight of loneliness can be crushing—it’s not just about being physically alone, but feeling like no one truly *sees* you. That isolation often distorts reality, making it hard to remember moments of connection or imagine reaching out. Right now, try this: Place a hand over your heart and notice your breath for 30 seconds. This simple act reminds your nervous system that *you* are here with yourself—and that matters. Loneliness thrives in silence, so if you can, consider one tiny breach in the barrier: a text to someone you’ve lost touch with, joining an online community about a niche interest, or even just making eye contact with a barista tomorrow. You don’t have to carry this forever. The fact that you shared this here tells me part of you still believes in connection—let’s nurture that part together.  
+Would it help to name one person (or pet, or memory) that once made you feel slightly less alone? We can start there.</t>
+  </si>
+  <si>
+    <t>I feel burnt out, like I’m constantly running on empty.</t>
+  </si>
+  <si>
+    <t>Feeling burnt out—like you're constantly running on empty—is a signal that your inner reserves have been depleted for too long without being replenished. Burnout isn’t just about being tired; it’s a deeper kind of exhaustion that touches your emotions, motivation, and even your sense of self. When you’ve been giving more than you’re receiving—whether emotionally, mentally, or physically—it eventually takes a toll, leaving you in survival mode. And in that place, even small tasks can feel like mountains. This isn’t a sign that you’re weak or failing; it’s a sign that you’ve been enduring more than your system was meant to carry alone. The hard part is that burnout often convinces you to just keep pushing, which only deepens the exhaustion. But healing begins when you give yourself permission to slow down, to say “no” even when it feels uncomfortable, and to reconnect with small things that nourish rather than drain. Can I ask—what does a typical day look like for you right now?</t>
+  </si>
+  <si>
+    <t>It sounds like you have been experiencing a lot of stress and emotional distress. It can be difficult to find healthy ways to cope, but it is important to keep trying. Have you considered talking to a therapist about these feelings? They can help you find ways to manage stress and improve your mental health.</t>
+  </si>
+  <si>
+    <t>I feel burnt out, like I’m constantly running on empty.
+That feeling of burnout, of constantly running on empty, is a significant sign that your resources are depleted. It's like your energy reserves have been consistently drawn upon without enough time for replenishment. This can manifest in various ways, not just as physical tiredness, but also as emotional exhaustion, a sense of detachment, and perhaps even a feeling of reduced accomplishment. Often, burnout creeps in gradually as a result of prolonged stress, excessive workload, or a mismatch between expectations and available support. Have you been noticing this feeling building over time, and are there specific areas of your life, like work or personal responsibilities, that feel particularly draining right now? Understanding the contributing factors can be the first step in finding ways to restore your energy and well-being.</t>
+  </si>
+  <si>
+    <t>Burnout develops gradually, like a slow leak that eventually leaves the tank empty, and it sounds like you've been operating in deficit for quite some time. When we continually override our body's signals for rest and replenishment, we enter a state where even basic functioning requires tremendous effort, and activities that once energized us may now feel like additional demands.
+Recovery from burnout isn't typically achieved through a single weekend of rest or one self-care activity. It requires a realistic reassessment of what you're carrying and permission to temporarily reduce your load. This might mean having difficult conversations about boundaries, letting go of certain responsibilities, or acknowledging that some things will need to remain undone for now. The path back from burnout often begins with small, intentional pauses throughout your day—brief moments to check in with yourself and respond to your needs before reaching complete depletion. 
+What's one responsibility or expectation that you might be able to temporarily adjust to create some breathing room?</t>
+  </si>
+  <si>
+    <t>Burnout is your body and mind’s way of sounding the alarm—it’s not a sign of failure, but a signal that your current pace is unsustainable. That "running on empty" feeling often comes from pushing forward while ignoring your limits, whether due to external pressures or internal expectations. Start by giving yourself permission to pause, even for five minutes. Ask: *What would rest look like if I didn’t have to earn it?* Small acts of resistance—like saying no to one non-essential task, or lying down without your phone—can begin to replenish you. Burnout thrives in cycles of guilt and overwork, so challenge the voice that says you *should* be able to handle it all. You’re a human being, not a machine. Let’s explore one tiny way you can prioritize your needs today—not because you’ve "done enough," but because you matter.  
+Would it help to identify what specifically feels most draining right now? (Work? Relationships? The mental load of daily life?) We can untangle it together.</t>
+  </si>
+  <si>
+    <t>I had a fight with someone close and now I feel horrible.</t>
+  </si>
+  <si>
+    <t>When you have a fight with someone close to you, it can feel like something inside you has cracked open. That kind of emotional conflict often brings up not just anger or frustration, but deep sadness, guilt, and fear—especially if the relationship really matters to you. Feeling horrible afterward is a sign that you care, and that the connection is important enough to hurt when it's disrupted. But it’s also important to remember that conflict, while painful, doesn’t automatically mean things are broken beyond repair. It can be a moment where something unspoken was brought to the surface. Sometimes we say things in defense that don’t reflect our deeper truth, and sometimes we hear things that trigger old wounds. It’s okay to feel awful—but try not to confuse that feeling with a final verdict. You’re allowed to take time to reflect and reconnect—both with yourself and the other person. Do you want to talk about what the fight was about, or how it ended?</t>
+  </si>
+  <si>
+    <t>It's understandable to feel horrible after a fight with someone close. Have you tried talking to the person to resolve the conflict? If not, it may be helpful to process your feelings with a therapist or counselor. Would you like me to find the nearest therapists for you?</t>
+  </si>
+  <si>
+    <t>It's completely understandable that you're feeling horrible after a fight with someone close to you. Conflicts with people we care about can be deeply upsetting and can trigger a range of difficult emotions, such as sadness, anger, guilt, or anxiety. The closeness of the relationship often amplifies these feelings because we value the connection and are sensitive to any ruptures in it. Could you tell me a little bit about the nature of the relationship and perhaps the general topic of the disagreement? Sometimes, understanding the context can help in processing the emotions that have come up. Remember, it's normal to have disagreements in close relationships, but the aftermath and how we navigate it are crucial for healing and repair.</t>
+  </si>
+  <si>
+    <t>The aftermath of conflict with someone important to us can create a particular kind of emotional undertow - that mix of regret, hurt, and unresolved tension that follows us even when we try to move on. That lingering distress you're feeling is actually a reflection of how much this relationship matters to you, even though the conflict itself feels terrible.
+When emotions are still raw, it's natural to replay the interaction and focus on what went wrong or what you could have said differently. This mental review serves a purpose in helping us process, but it can also keep the wound fresh. Consider that most meaningful relationships can withstand disagreement and repair after conflict - sometimes emerging stronger for having navigated difficult territory together. Once the immediate emotional intensity subsides, reaching out with even a simple acknowledgment of the tension can often begin shifting things toward resolution, whether that means clarifying misunderstandings or simply confirming that the relationship remains important despite the disagreement.
+What do you think would feel like a manageable first step toward easing this tension, even if it doesn't immediately resolve everything?</t>
+  </si>
+  <si>
+    <t>Conflict with someone we care about can leave you feeling physically sick—that ache in your chest, the racing thoughts replaying what was said or what you "should have" done differently. It’s important to recognize: this discomfort means the relationship matters to you, not that you’ve ruined it. Right now, try to separate the feeling (hurt, guilt, shame) from the facts (one argument doesn’t define the entire connection). If possible, give yourself space to cool off before re-engaging—write down what you’re feeling (unsent letters can be cathartic) or move your body to release the tension. Later, you can revisit the conversation with clarity. Repair is always possible when both people are willing. For now, though, tend to your wounds like you would a friend’s.
+If it feels safe: What’s one small step toward repair—or self-kindness—you could take today?</t>
+  </si>
+  <si>
+    <t>My mood is constantly bad and I feel angry all the time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Living with a persistently bad mood and frequent anger can be exhausting—it’s like your emotional baseline is set to frustration, and even small things can feel triggering or overwhelming. Anger is often misunderstood; while it can be loud and outward, it’s also frequently a mask for other emotions—hurt, fear, helplessness, grief, or unmet needs that haven’t had space to be seen. When you're stuck in that angry state, it can feel like you’re on edge all the time, defensive before anything even happens, and sometimes guilty afterward for how you reacted. But this doesn’t mean you’re a bad person—it means something inside you has likely gone unheard or unhealed for a long time. Chronic anger is often a sign that your emotional system is overburdened and craving relief, boundaries, or understanding. What do you think might be fueling the anger beneath the surface—are there people, situations, or thoughts that seem to light the fuse more quickly lately?
+</t>
+  </si>
+  <si>
+    <t>It sounds like you are dealing with a lot of difficult emotions and are struggling to control your anger. It may be helpful to seek out a therapist or counselor who can provide you with coping techniques and support to manage your anger in a healthy way. Would you like me to find the nearest therapists for you?</t>
+  </si>
+  <si>
+    <t>My mood is constantly bad and I feel angry all the time.
+It sounds really distressing to be experiencing a consistently low mood and frequent anger. Living in a state of constant negativity can be incredibly draining and impact various aspects of your life, from your relationships to your overall well-being. This persistent anger might be a primary emotion you're aware of, but sometimes anger can also act as a surface emotion, masking other underlying feelings like sadness, frustration, or fear. Have you noticed any patterns or triggers that seem to exacerbate these feelings of low mood and anger? Are there specific times of day or situations where these feelings tend to be more intense? Exploring these patterns could offer some insight into what might be contributing to this persistent state. It's important to remember that these intense and persistent emotions are signals, and understanding them better can be the first step towards finding more balanced and positive emotional states.</t>
+  </si>
+  <si>
+    <t>Persistent anger often functions as a protective emotion that rises to the surface when deeper feelings - like hurt, fear, or powerlessness - feel too vulnerable to experience directly. Living with this constant internal tension is exhausting, like carrying a heavy weight that never gets put down, and it can color everything from how you interpret others' actions to how you experience everyday situations.
+This ongoing irritability typically signals that something important in your life needs attention - perhaps boundaries that need strengthening, needs that aren't being met, or past experiences that haven't been fully processed. While anger itself isn't inherently problematic, when it becomes your primary emotional state, it can isolate you from potential sources of support and make it difficult to identify what might actually help. Consider checking in with your body when anger surfaces - where you feel it physically and whether there might be other emotions beneath it asking for recognition.
+What tends to happen just before you notice your anger intensifying? Those triggers sometimes offer clues about what's actually feeding this emotional state.</t>
+  </si>
+  <si>
+    <t>What you're describing—that constant undercurrent of anger and low mood—sounds exhausting to carry. Anger often acts as a protective layer, covering deeper emotions like hurt, helplessness, or unmet needs. Instead of judging the anger (which usually makes it louder), try getting curious with it. *Where does this feel strongest in my body? What might it be trying to tell me?* Sometimes just naming it—"I’m feeling rage because I’m overwhelmed and no one notices"—can take the edge off.  
+Consider whether this anger might be linked to something specific (a life circumstance, unresolved grief) or if it’s more generalized (a sign of depression or chronic stress). Either way, your system is asking for attention. Small releases—screaming into a pillow, tearing up paper, or intense exercise—can help discharge the physical tension. Longer term, we might explore boundaries, unmet needs, or even physiological factors like sleep or hormones. You deserve relief from this weight.  
+Would you be open to experimenting with one healthy outlet this week? (Even something simple like scribbling in a notebook until your hand cramps?)</t>
+  </si>
+  <si>
+    <t>Feeling burnt out and constantly running on empty can make even the simplest things feel unbearable. It’s not just tiredness—it’s a deep, soul-level depletion, where you’re giving more than you’re receiving, and rest never feels truly restorative. Burnout often comes from prolonged stress, emotional strain, or being in situations where you feel like you can’t stop, slow down, or ask for help. It’s common to keep pushing because you feel you have to—but eventually, that catches up with you, and your mind and body start sending warning signs. Feeling disconnected, irritable, or numb are all part of that picture. It’s important to recognize that this isn’t your fault, and it doesn’t mean you’re weak—it means you’re human. You may need more rest, more space, or a chance to re-evaluate what’s draining you. Has anything changed recently in your work, relationships, or responsibilities that might be contributing to this feeling?</t>
+  </si>
+  <si>
+    <t>It sounds like you may be experiencing burnout. Burnout is a state of emotional, physical, and mental exhaustion caused by excessive and prolonged stress. It's important to take care of yourself and prioritize self-care during this time. Have you considered talking to a therapist about how you are feeling? They can provide you with personalized support and guidance to help you manage your stress and improve your well-being.</t>
+  </si>
+  <si>
+    <t>It sounds like you're describing a state of significant depletion, where you feel like you have very little energy to draw upon. This feeling of being constantly on empty, often referred to as burnout, can be really challenging as it impacts not just your physical energy but also your emotional and mental reserves. It often arises from prolonged periods of stress or feeling overwhelmed without adequate opportunity for rest and recovery.
+Given that you mentioned this feeling earlier today as well, it seems like this is an ongoing experience for you. Have you noticed if there are particular aspects of your life – perhaps work, personal responsibilities, or social engagements – that feel particularly draining or contribute most to this sense of being burnt out? Sometimes identifying the key stressors can help in figuring out strategies to address them and begin to replenish your energy levels. Remember, it's important to prioritize rest and self-care when you're feeling this way, even if it feels difficult to find the time or energy for it.</t>
+  </si>
+  <si>
+    <t>I'm sorry to hear you're feeling burnt out. That sensation of "running on empty" can be really difficult to manage, both physically and emotionally.
+Would you mind sharing a bit more about what's contributing to your burnout? Sometimes it can be work-related, other times it might be personal obligations, or often a combination of many factors. Understanding the specific sources might help us talk through some potential approaches to help you recover.
+In the meantime, have you been able to take any breaks or moments for yourself recently? Even small pauses can sometimes help when you're feeling completely depleted.</t>
+  </si>
+  <si>
+    <t>Burnout is your body’s way of forcing you to listen when you’ve pushed too hard for too long. That "running on empty" feeling isn’t a personal failing—it’s a sign that your current pace is unsustainable. Start by questioning the invisible rules driving you: Who told me I had to keep going like this? What would happen if I truly rested? The exhaustion isn’t just physical; it’s often a soul-deep weariness from neglecting your own needs while tending to others’ demands.
+For now, focus on micro-rest: Set a timer for two minutes and stare out a window. Leave one chore undone today. Say no to the next non-essential ask. Burnout thrives in the myth that you must earn rest, so rebel against that. Your worth isn’t tied to your productivity. Let’s explore what refueling (not just recovering) could look like for you—what’s one thing that used to bring you lightness, even years ago? We can start there.
+This isn’t just about surviving—it’s about reclaiming yourself.</t>
+  </si>
+  <si>
+    <t>What’s the point of anything anymore?</t>
+  </si>
+  <si>
+    <t>When you find yourself asking, “What’s the point of anything anymore?” it often means something inside you is deeply worn down, disillusioned, or grieving. It’s a question that doesn’t come from indifference—it comes from pain, from exhaustion, from the quiet hope that life should feel more meaningful than it does right now. In these moments, your world can feel colorless, like you’re going through the motions but none of it touches you. This kind of emptiness is incredibly hard, and it can make everything—your past, your future, even your daily routine—feel like it has no weight or purpose.
+But here’s what’s still true, even if you can’t feel it right now: the absence of meaning in this moment doesn’t mean your life is meaningless. Meaning is something that can dim, go dormant, or feel buried under everything you’ve been carrying—but it doesn’t disappear. Often, it’s not about finding a grand purpose, but about reconnecting with small things that remind you you’re alive and still human—quiet moments, honest conversations, even this one right now.
+You don’t have to figure out the whole point of life today. Right now, it’s enough to just not turn away from the question. What’s making the world feel so pointless for you lately?</t>
+  </si>
+  <si>
+    <t>The meaning of life is subjective and can vary from person to person. Some may find meaning in their relationships, others in their work or hobbies, and some may find it in spirituality or personal growth. It's important to explore and discover what brings meaning and purpose to your own life. Have you considered talking to a therapist about these existential thoughts? They can help guide you in finding your own sense of purpose and fulfillment.</t>
+  </si>
+  <si>
+    <t>That's a profound question, and it's one that many people grapple with at different times in their lives, especially when feeling overwhelmed or disconnected. When you ask, "What's the point of anything anymore?" it sounds like you might be experiencing a sense of meaninglessness or a lack of purpose in your current circumstances. This feeling can be really disheartening and can make it difficult to find motivation or joy in daily life.
+Sometimes, this feeling can arise from significant life changes, ongoing stress, or even an internal shift in perspective. It might be helpful to gently explore what aspects of your life currently feel like they lack meaning. Are there things you used to find fulfilling that no longer do? Have there been any recent events that have shifted your perspective on what's important?
+It's also worth remembering that the "point" of things isn't always a fixed or universal answer. Sometimes, meaning and purpose are things we actively create and discover through our experiences, our connections with others, and our values. Exploring what truly matters to you, even in small ways, might be a starting point in reconnecting with a sense of purpose.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That's a profound question that many people wrestle with at various points in their lives. It touches on some of the deepest aspects of human existence.
+The "point" or meaning of life isn't something that's universally defined or given to us—it's often something we create or discover for ourselves. Different people find purpose in different ways:
+Connections with others: The relationships we build, love we share, and impact we have on those around us
+Personal growth: Learning, overcoming challenges, and becoming more of who we want to be
+Contributing to something larger: Whether that's family, community, causes, or humanity as a whole
+Finding joy and wonder: Appreciating beauty, experiencing new things, or simply being present in moments of contentment
+Is there something specific that's prompted this question for you? Sometimes these thoughts arise during difficult periods, when we're feeling disconnected, or when facing significant life </t>
+  </si>
+  <si>
+    <t>That question—What’s the point?—is the heavy fog that rolls in when exhaustion, pain, or isolation cloud your vision. It’s not a truth, but a sign that your emotional reserves are depleted. When the brain is worn down, it struggles to imagine a future that feels different from the present. But meaning isn’t something you find—it’s something you rebuild, one small brick at a time.
+Start here: When have I felt even flickers of purpose before? Maybe it was caring for a pet, creating something, or a moment of quiet under the sky. You don’t need a grand reason to exist—you’re allowed to be here simply because you are. For now, strip it down to the basics: Drink water. Sit where sunlight touches your skin. Text someone who once made you feel less alone. The fog will lift enough for you to see the next step, and the next.
+I know it feels impossible right now, but you’ve survived every bad day so far. Let’s keep going—together. Would you be willing to try one tiny act of rebellion against the emptiness today? (Even just opening a window counts.)</t>
   </si>
 </sst>
 </file>
@@ -168,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -184,9 +448,6 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,7 +661,12 @@
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1" pane="topRight"/>
+      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
+      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
@@ -514,20 +780,224 @@
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="A6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="7">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="A7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+      <c r="A8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>